<commit_message>
#108 don't call getRunVar with null
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue93Test.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue93Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\JobStuff\GitRepos\jxls\jxls-poi\src\test\resources\org\jxls\templatebasedtests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BAA882-8C4E-4D4F-A167-440584230593}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA9962-4756-437D-90D5-1E918303F985}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B60A3C6-E657-4C54-B244-F7E7FF287A0C}"/>
   </bookViews>
@@ -87,12 +87,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6842922E-2D18-4646-9B64-60DD4C9300A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jxlsteam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="list2" var="m" lastCell="B7")</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>${e}</t>
   </si>
@@ -110,6 +134,9 @@
   </si>
   <si>
     <t>${i+1}</t>
+  </si>
+  <si>
+    <t>${m}</t>
   </si>
 </sst>
 </file>
@@ -521,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3623DDB8-F445-4CED-AB60-642E6F741FD0}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +580,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#108 don't call getRunVar with null (#109)
* #108 don't call getRunVar with null

* RC2

* fixed EachCommandTest
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue93Test.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue93Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\JobStuff\GitRepos\jxls\jxls-poi\src\test\resources\org\jxls\templatebasedtests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BAA882-8C4E-4D4F-A167-440584230593}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA9962-4756-437D-90D5-1E918303F985}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B60A3C6-E657-4C54-B244-F7E7FF287A0C}"/>
   </bookViews>
@@ -87,12 +87,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6842922E-2D18-4646-9B64-60DD4C9300A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jxlsteam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="list2" var="m" lastCell="B7")</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>${e}</t>
   </si>
@@ -110,6 +134,9 @@
   </si>
   <si>
     <t>${i+1}</t>
+  </si>
+  <si>
+    <t>${m}</t>
   </si>
 </sst>
 </file>
@@ -521,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3623DDB8-F445-4CED-AB60-642E6F741FD0}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +580,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>